<commit_message>
Implement activeSheet + activeCell + worksheetView
</commit_message>
<xml_diff>
--- a/tests/documents/multi.xlsx
+++ b/tests/documents/multi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,9 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>simple</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>multi</t>
   </si>
   <si>
     <t>read</t>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>!</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -136,12 +139,12 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -174,17 +177,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="B1:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="10.8010204081633"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>